<commit_message>
new template - added blackout dates
</commit_message>
<xml_diff>
--- a/data/TT/Coach-2020.xlsx
+++ b/data/TT/Coach-2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\DjangoLeagueScheduler\data\9-29-19_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\DjangoLeagueScheduler\data\TT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BBD560-A548-4AE5-BAD4-50F699456061}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514B5120-E88B-4343-A5ED-BB95AD974740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="30" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19632" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablib Dataset" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Coach G</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
@@ -411,16 +417,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -442,7 +448,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2</v>
       </c>
@@ -453,7 +459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>3</v>
       </c>
@@ -464,7 +470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>4</v>
       </c>
@@ -475,7 +481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>5</v>
       </c>
@@ -486,7 +492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>6</v>
       </c>
@@ -495,6 +501,17 @@
       </c>
       <c r="C7" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>